<commit_message>
- Models for Torch Added with Measurement Sheets, Updated Completion List
</commit_message>
<xml_diff>
--- a/Models/Kelly's Models/Model_TO_DO_List_and_Completion_Tracker.xlsx
+++ b/Models/Kelly's Models/Model_TO_DO_List_and_Completion_Tracker.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
   <si>
     <t>Model Name</t>
   </si>
@@ -61,6 +61,105 @@
   </si>
   <si>
     <t>Large Decorative Door Frame.</t>
+  </si>
+  <si>
+    <t>Wall_Solid</t>
+  </si>
+  <si>
+    <t>Wall_Cutout</t>
+  </si>
+  <si>
+    <t>Wall_Cutout_Flipped</t>
+  </si>
+  <si>
+    <t>Wall_Cutout_Accents</t>
+  </si>
+  <si>
+    <t>Wall_Cutout_Flipped_Accents</t>
+  </si>
+  <si>
+    <t>Molding_Floor</t>
+  </si>
+  <si>
+    <t>Molding_Ceiling</t>
+  </si>
+  <si>
+    <t>Single Panel of Stone Brick Wall.</t>
+  </si>
+  <si>
+    <t>Single Panel of Stone Brick Wall with a trapizoid (small side on bottom) shaped built in alcove.</t>
+  </si>
+  <si>
+    <t>Single Panel of Stone Brick Wall with a trapizoid (small side on top) shaped built in alcove.</t>
+  </si>
+  <si>
+    <t>Single Panel of Stone Brick Wall with a trapizoid (small side on top) shaped built in alcove. Stone accents around the small edge of the trapizoid alcove.</t>
+  </si>
+  <si>
+    <t>Single Panel of Stone Brick Wall with a trapizoid (small side on bottom) shaped built in alcove. Stone accents around the small edge of the trapizoid alcove.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angular shaped molding that can be placed in front of a wall panel against the floor, to add accent to it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angular shaped molding that can be placed in front of a wall panel, against the ceiling, to add accent to it. </t>
+  </si>
+  <si>
+    <t>Column_Top</t>
+  </si>
+  <si>
+    <t>Column_Bottom</t>
+  </si>
+  <si>
+    <t>Column_Center</t>
+  </si>
+  <si>
+    <t>The bottom piece of a free standing pillar.</t>
+  </si>
+  <si>
+    <t>The center piece of a free standing pillar, to increase height of pillar add additional center pieces.</t>
+  </si>
+  <si>
+    <t>The top piece of a free standing pillar.</t>
+  </si>
+  <si>
+    <t>Furniture</t>
+  </si>
+  <si>
+    <t>Table_Solid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solid stone table, can be used as an altar, or table in any room. </t>
+  </si>
+  <si>
+    <t>Wall_Column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Half of a column meant to be placed against a wall for accent purposes. </t>
+  </si>
+  <si>
+    <t>Stairs_Steps</t>
+  </si>
+  <si>
+    <t>Steps of a staircase can be stacked to extend side of the stairs.</t>
+  </si>
+  <si>
+    <t>Stairs_Edges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decorative stone edging to be used with smaller sets of stairs. </t>
+  </si>
+  <si>
+    <t>Torch_Pillar</t>
+  </si>
+  <si>
+    <t>Torch_Bowl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A stone pillar that holds a bowl which is meant to have a fire lit in it for lighting a room. </t>
+  </si>
+  <si>
+    <t>The bowl of a torch, placed on top of a pillar or nearby on the ground if the pillar is broken.</t>
   </si>
 </sst>
 </file>
@@ -129,16 +228,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -151,6 +262,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,65 +580,416 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" s="9" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="10">
         <v>876</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2">
+        <v>232</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2">
+        <v>242</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <v>242</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2">
+        <v>18</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2">
+        <v>250</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2">
+        <v>18</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2">
+        <v>50</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2">
+        <v>598</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="2">
+        <v>936</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="2">
+        <v>512</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- All current models uploaded, with some measurement sheets.
</commit_message>
<xml_diff>
--- a/Models/Kelly's Models/Model_TO_DO_List_and_Completion_Tracker.xlsx
+++ b/Models/Kelly's Models/Model_TO_DO_List_and_Completion_Tracker.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
   <si>
     <t>Model Name</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>The bowl of a torch, placed on top of a pillar or nearby on the ground if the pillar is broken.</t>
+  </si>
+  <si>
+    <t>Torch</t>
+  </si>
+  <si>
+    <t>Combination of Torch_Bowl and Torch_Pillar</t>
   </si>
 </sst>
 </file>
@@ -580,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,8 +771,8 @@
       <c r="D8" s="2">
         <v>18</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>10</v>
+      <c r="E8" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>8</v>
@@ -990,6 +996,29 @@
         <v>8</v>
       </c>
       <c r="G18" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1448</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Added accented walls, started on wall column
</commit_message>
<xml_diff>
--- a/Models/Kelly's Models/Model_TO_DO_List_and_Completion_Tracker.xlsx
+++ b/Models/Kelly's Models/Model_TO_DO_List_and_Completion_Tracker.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
   <si>
     <t>Model Name</t>
   </si>
@@ -63,21 +63,6 @@
     <t>Large Decorative Door Frame.</t>
   </si>
   <si>
-    <t>Wall_Solid</t>
-  </si>
-  <si>
-    <t>Wall_Cutout</t>
-  </si>
-  <si>
-    <t>Wall_Cutout_Flipped</t>
-  </si>
-  <si>
-    <t>Wall_Cutout_Accents</t>
-  </si>
-  <si>
-    <t>Wall_Cutout_Flipped_Accents</t>
-  </si>
-  <si>
     <t>Molding_Floor</t>
   </si>
   <si>
@@ -165,14 +150,47 @@
     <t>Torch</t>
   </si>
   <si>
-    <t>Combination of Torch_Bowl and Torch_Pillar</t>
+    <t>Wall_Panel_Solid</t>
+  </si>
+  <si>
+    <t>Wall_Panel_Cutout</t>
+  </si>
+  <si>
+    <t>Wall_Panel_Cutout_Flipped</t>
+  </si>
+  <si>
+    <t>Wall_Panel_Cutout_Accents</t>
+  </si>
+  <si>
+    <t>Wall_Panel_Cutout_Flipped_Accents</t>
+  </si>
+  <si>
+    <t>Ceilling_Panels</t>
+  </si>
+  <si>
+    <t>Flooring_Panels</t>
+  </si>
+  <si>
+    <t>Combination of Torch_Bowl and Torch_Pillar with proper placement.</t>
+  </si>
+  <si>
+    <t>Stone_Throne_Ornate</t>
+  </si>
+  <si>
+    <t>Table_With_Legs</t>
+  </si>
+  <si>
+    <t>Fountain_Water_Spout</t>
+  </si>
+  <si>
+    <t>STARTED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +218,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -234,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -271,6 +297,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,20 +679,20 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
+      <c r="A3" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2">
         <v>232</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>10</v>
+      <c r="E3" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>8</v>
@@ -674,19 +703,19 @@
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2">
         <v>242</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>10</v>
+      <c r="E4" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>8</v>
@@ -697,19 +726,19 @@
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2">
         <v>242</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>10</v>
+      <c r="E5" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>8</v>
@@ -720,19 +749,22 @@
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="2">
+        <v>442</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>10</v>
@@ -740,19 +772,22 @@
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="D7" s="2">
+        <v>442</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>10</v>
@@ -760,13 +795,13 @@
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2">
         <v>18</v>
@@ -783,13 +818,13 @@
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>10</v>
@@ -803,13 +838,13 @@
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="D10" s="2">
         <v>250</v>
@@ -826,13 +861,13 @@
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2">
         <v>18</v>
@@ -849,13 +884,13 @@
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D12" s="2">
         <v>50</v>
@@ -872,13 +907,13 @@
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D13" s="2">
         <v>598</v>
@@ -895,19 +930,19 @@
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>10</v>
+      <c r="F14" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>10</v>
@@ -915,13 +950,13 @@
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>10</v>
@@ -935,13 +970,13 @@
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>10</v>
@@ -955,13 +990,13 @@
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2">
         <v>936</v>
@@ -978,13 +1013,13 @@
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2">
         <v>512</v>
@@ -1001,13 +1036,13 @@
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D19" s="2">
         <v>1448</v>
@@ -1019,6 +1054,91 @@
         <v>8</v>
       </c>
       <c r="G19" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Added model & measurement sheet for columns that are placed against the walls, updated completion tracker, additional working files.
</commit_message>
<xml_diff>
--- a/Models/Kelly's Models/Model_TO_DO_List_and_Completion_Tracker.xlsx
+++ b/Models/Kelly's Models/Model_TO_DO_List_and_Completion_Tracker.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="52">
   <si>
     <t>Model Name</t>
   </si>
@@ -181,16 +180,13 @@
   </si>
   <si>
     <t>Fountain_Water_Spout</t>
-  </si>
-  <si>
-    <t>STARTED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,14 +214,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -260,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -297,9 +285,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -618,7 +603,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,11 +923,14 @@
       <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>52</v>
+      <c r="D14" s="2">
+        <v>254</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>10</v>

</xml_diff>